<commit_message>
Commit: 8.0 - Excel parser and pom update using Apache POI dependencies
</commit_message>
<xml_diff>
--- a/src/test/resources/basicRessources/TestData.xlsx
+++ b/src/test/resources/basicRessources/TestData.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1f443580377edc98/Documents/gitDevelopmentTesting/SeleniumRestNG/src/test/resources/basicRessources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="11_F25DC773A252ABDACC1048A2615D55C65ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6FB7EE7-911C-4052-A3A6-55AC019A5567}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:801_{C2CA3E8F-19A6-4FCF-8B03-DB1C5371C0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6FD8FC4-1098-4F77-898F-D6B63C182721}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2676" yWindow="1584" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RegistrationForm" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Registration details</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Login Data</t>
+  </si>
+  <si>
+    <t>1998,Jan,1</t>
   </si>
 </sst>
 </file>
@@ -500,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,8 +557,8 @@
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4">
-        <v>35916</v>
+      <c r="B6" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -649,7 +652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A47F7997-0EC9-4133-BF9E-BF22FD5E38B5}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Completed the basic development of step definition
</commit_message>
<xml_diff>
--- a/src/test/resources/basicRessources/TestData.xlsx
+++ b/src/test/resources/basicRessources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1f443580377edc98/Documents/gitDevelopmentTesting/SeleniumRestNG/src/test/resources/basicRessources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:801_{C2CA3E8F-19A6-4FCF-8B03-DB1C5371C0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6FD8FC4-1098-4F77-898F-D6B63C182721}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:801_{A322A9FA-3311-4E9B-A085-EF8C30FBCFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B80DB82D-CFAB-4F8E-8EB2-2ACA0E624939}"/>
   <bookViews>
     <workbookView xWindow="2676" yWindow="1584" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,26 @@
     <sheet name="RegistrationForm" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Registration details</t>
   </si>
@@ -133,7 +142,19 @@
     <t>Login Data</t>
   </si>
   <si>
-    <t>1998,Jan,1</t>
+    <t>Number:9999999999</t>
+  </si>
+  <si>
+    <t>PIN:500019</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>1998:January:1</t>
   </si>
 </sst>
 </file>
@@ -173,7 +194,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -196,12 +217,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -220,6 +252,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -501,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,7 +596,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -627,16 +665,24 @@
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="5">
-        <v>500019</v>
+      <c r="B15" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="5">
-        <v>9999999999</v>
+      <c r="B16" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>